<commit_message>
update api function list
</commit_message>
<xml_diff>
--- a/api_function_list.xlsx
+++ b/api_function_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="200">
   <si>
     <t>NO.</t>
   </si>
@@ -77,19 +77,10 @@
     <t>Forget pass</t>
   </si>
   <si>
-    <t>api/account/forget-pass</t>
-  </si>
-  <si>
-    <t>Quên mật khẩu -&gt; confirm code</t>
-  </si>
-  <si>
     <t>Customer confirm code to active account</t>
   </si>
   <si>
     <t>Customer confirm code to update pass</t>
-  </si>
-  <si>
-    <t>api/account/update-pass</t>
   </si>
   <si>
     <t>Quét QR code</t>
@@ -602,6 +593,48 @@
   </si>
   <si>
     <t>{"phone_number": "0976111444", "password": "123456"}</t>
+  </si>
+  <si>
+    <t>{"id": 11,"code": "3080"}</t>
+  </si>
+  <si>
+    <t>api/customer/update-pass</t>
+  </si>
+  <si>
+    <t>api/customer/active-pass</t>
+  </si>
+  <si>
+    <t>{
+ "phone_number": "0977777444"
+ ,"new_pass": "111111"
+}</t>
+  </si>
+  <si>
+    <t>{
+ "phone_number": "0977777444"
+ ,"code": "2604"
+}</t>
+  </si>
+  <si>
+    <t>Staff quên mật khẩu</t>
+  </si>
+  <si>
+    <t>api/staff/update-pass</t>
+  </si>
+  <si>
+    <t>Customer quên mật khẩu -&gt; confirm code</t>
+  </si>
+  <si>
+    <t>Customer quên mật khẩu</t>
+  </si>
+  <si>
+    <t>Staff quên mật khẩu -&gt; confirm code</t>
+  </si>
+  <si>
+    <t>Staff confirm code to update pass</t>
+  </si>
+  <si>
+    <t>api/staff/active-pass</t>
   </si>
 </sst>
 </file>
@@ -802,6 +835,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -852,9 +888,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1160,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G14"/>
+  <dimension ref="A2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1226,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>4</v>
@@ -1216,10 +1249,10 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1239,10 +1272,10 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G4" t="s">
         <v>187</v>
-      </c>
-      <c r="G4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1262,10 +1295,10 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>187</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1276,7 +1309,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -1284,13 +1317,19 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>184</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>196</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1299,103 +1338,151 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="F7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="F8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="F9" t="s">
+        <v>184</v>
+      </c>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>29</v>
+        <v>197</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="F10" t="s">
+        <v>184</v>
+      </c>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
       <c r="E14" t="s">
-        <v>188</v>
-      </c>
-      <c r="F14" t="s">
-        <v>187</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>189</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" t="s">
+        <v>184</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +1495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AJ122"/>
   <sheetViews>
-    <sheetView topLeftCell="I71" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -1427,130 +1514,130 @@
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="T5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="U5" s="3"/>
       <c r="W5" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Y5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AG5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="AH5" s="3"/>
       <c r="AJ5" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AH6" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Y7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="M9" t="s">
         <v>45</v>
       </c>
-      <c r="M9" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q9" s="22"/>
+      <c r="P9" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q9" s="23"/>
       <c r="Y9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB9" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="AB9" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AB10" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1558,32 +1645,32 @@
         <v>14</v>
       </c>
       <c r="M11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P11" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z11" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA11" s="22"/>
+        <v>62</v>
+      </c>
+      <c r="Z11" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA11" s="23"/>
     </row>
     <row r="12" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P12" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M13" t="s">
-        <v>51</v>
-      </c>
-      <c r="P13" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q13" s="22"/>
+        <v>48</v>
+      </c>
+      <c r="P13" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q13" s="23"/>
     </row>
     <row r="14" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="2" t="s">
@@ -1592,48 +1679,48 @@
     </row>
     <row r="15" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M15" t="s">
-        <v>52</v>
-      </c>
-      <c r="P15" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q15" s="22"/>
+        <v>49</v>
+      </c>
+      <c r="P15" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q15" s="23"/>
     </row>
     <row r="16" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P20" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1643,89 +1730,89 @@
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="V23" s="1"/>
     </row>
     <row r="24" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H24" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="E25" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="25"/>
+      <c r="H25" t="s">
+        <v>179</v>
+      </c>
+      <c r="L25" t="s">
         <v>83</v>
-      </c>
-      <c r="C25" s="24"/>
-      <c r="E25" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="24"/>
-      <c r="H25" t="s">
-        <v>182</v>
-      </c>
-      <c r="L25" t="s">
-        <v>86</v>
       </c>
       <c r="N25">
         <v>300000</v>
       </c>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
       <c r="D26" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="26"/>
+        <v>91</v>
+      </c>
+      <c r="E26" s="26"/>
+      <c r="F26" s="27"/>
       <c r="H26" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="27"/>
       <c r="H27" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29"/>
       <c r="L28">
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O28">
         <v>3000</v>
       </c>
       <c r="Q28" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R28" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="S28" s="3">
         <v>0</v>
@@ -1736,46 +1823,46 @@
         <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O29">
         <v>4000</v>
       </c>
       <c r="Q29" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R29" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="S29" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="22"/>
+      <c r="B30" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="23"/>
     </row>
     <row r="31" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
@@ -1789,13 +1876,13 @@
     </row>
     <row r="35" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1803,46 +1890,46 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E36">
         <v>55000</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I36" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J36" s="22"/>
+        <v>75</v>
+      </c>
+      <c r="I36" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J36" s="23"/>
     </row>
     <row r="37" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E37">
         <v>30000</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I37" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J37" s="22"/>
+        <v>75</v>
+      </c>
+      <c r="I37" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J37" s="23"/>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G39" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
@@ -1869,123 +1956,123 @@
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C49" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="14"/>
+      <c r="C49" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="15"/>
     </row>
     <row r="50" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C50" s="15"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="17"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="18"/>
     </row>
     <row r="51" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C51" s="15"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="17"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="18"/>
     </row>
     <row r="52" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="18"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="20"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="21"/>
     </row>
     <row r="55" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="D57" s="22"/>
+      <c r="C57" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" s="23"/>
       <c r="G57" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="T57" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K58" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="22"/>
+      <c r="C59" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" s="23"/>
       <c r="U59" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N60" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C61" s="21" t="s">
+      <c r="C61" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" s="23"/>
+      <c r="F61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G61" t="s">
         <v>101</v>
       </c>
-      <c r="D61" s="22"/>
-      <c r="F61" t="s">
-        <v>74</v>
-      </c>
-      <c r="G61" t="s">
-        <v>104</v>
-      </c>
       <c r="H61" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I61" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="P61" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q61" s="5"/>
       <c r="V61" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1993,129 +2080,129 @@
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H62">
         <v>30000</v>
       </c>
       <c r="I62" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K62" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L62" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="N62" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C63" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D63" s="22"/>
+      <c r="C63" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D63" s="23"/>
       <c r="F63">
         <v>2</v>
       </c>
       <c r="G63" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H63">
         <v>20000</v>
       </c>
       <c r="I63" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K63" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L63" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="P63" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="V63" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="X63" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N64" t="s">
+        <v>111</v>
+      </c>
+      <c r="P64" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q64" s="23"/>
+      <c r="R64" t="s">
         <v>114</v>
-      </c>
-      <c r="P64" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q64" s="22"/>
-      <c r="R64" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="65" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R65" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P66" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="6:25" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G71" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="U71" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K72" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P73" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R73" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="V73" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="74" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F74" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G74" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J74" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K74" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="R74" s="5"/>
       <c r="S74" s="5"/>
@@ -2125,104 +2212,104 @@
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J75" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K75" s="7">
         <v>43821</v>
       </c>
       <c r="M75" t="s">
+        <v>129</v>
+      </c>
+      <c r="N75" t="s">
+        <v>130</v>
+      </c>
+      <c r="P75" t="s">
+        <v>38</v>
+      </c>
+      <c r="R75" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="W75" t="s">
         <v>132</v>
-      </c>
-      <c r="N75" t="s">
-        <v>133</v>
-      </c>
-      <c r="P75" t="s">
-        <v>41</v>
-      </c>
-      <c r="R75" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="W75" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="76" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R76" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P77" t="s">
-        <v>125</v>
-      </c>
-      <c r="R77" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="S77" s="22"/>
+        <v>122</v>
+      </c>
+      <c r="R77" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="S77" s="23"/>
       <c r="W77" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Y77" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="79" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q79" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G81" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P81" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="U81" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K82" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P83" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R83" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="V83" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F84" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G84" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H84" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I84" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K84" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="R84" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="S84" s="5"/>
     </row>
@@ -2231,7 +2318,7 @@
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H85">
         <v>1000</v>
@@ -2243,170 +2330,170 @@
         <v>43730</v>
       </c>
       <c r="M85" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N85" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="P85" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R85" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="W85" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="86" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R86" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P87" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="R87" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="T87" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="W87" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Y87" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="2:25" x14ac:dyDescent="0.25">
       <c r="R88" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="90" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G90" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q90" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="91" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K91" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="92" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="93" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G93" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K93" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="96" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G96" s="9"/>
     </row>
     <row r="97" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="98" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C98" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="D98" s="22"/>
+      <c r="C98" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D98" s="23"/>
       <c r="F98" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N98" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="R98" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="X98" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C100" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="D100" s="22"/>
+      <c r="C100" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D100" s="23"/>
       <c r="F100" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G100" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="I100" t="s">
+        <v>151</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="M100" t="s">
         <v>152</v>
       </c>
-      <c r="I100" t="s">
-        <v>154</v>
-      </c>
-      <c r="K100" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="M100" t="s">
-        <v>155</v>
-      </c>
       <c r="N100" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="R100" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="T100" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Y100" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="102" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N102" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="R102" t="s">
-        <v>51</v>
-      </c>
-      <c r="T102" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="U102" s="22"/>
+        <v>48</v>
+      </c>
+      <c r="T102" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="U102" s="23"/>
       <c r="Z102" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="103" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F103" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G103" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H103" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J103" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K103" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="L103" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N103" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="104" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2414,16 +2501,16 @@
         <v>1</v>
       </c>
       <c r="G104" t="s">
+        <v>154</v>
+      </c>
+      <c r="H104" t="s">
+        <v>155</v>
+      </c>
+      <c r="J104" t="s">
+        <v>156</v>
+      </c>
+      <c r="K104" t="s">
         <v>157</v>
-      </c>
-      <c r="H104" t="s">
-        <v>158</v>
-      </c>
-      <c r="J104" t="s">
-        <v>159</v>
-      </c>
-      <c r="K104" t="s">
-        <v>160</v>
       </c>
       <c r="L104" s="7">
         <v>44187</v>
@@ -2432,130 +2519,130 @@
         <v>43821</v>
       </c>
       <c r="P104" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Q104" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="R104" t="s">
-        <v>52</v>
-      </c>
-      <c r="T104" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="U104" s="22"/>
+        <v>49</v>
+      </c>
+      <c r="T104" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="U104" s="23"/>
       <c r="Z104" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="AB104" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="105" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="106" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R106" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="T106" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="X106" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="107" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="108" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R108" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="T108" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="V108" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="109" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="110" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T110" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="111" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="112" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F112" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O112" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="R112" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="X112" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="114" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F114" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I114" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M114" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O114" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="R114" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="T114" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Y114" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="116" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O116" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="R116" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="T116" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Z116" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="117" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F117" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G117" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H117" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J117" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K117" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2563,53 +2650,53 @@
         <v>1</v>
       </c>
       <c r="G118" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H118" s="8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J118" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K118" s="7">
         <v>43821</v>
       </c>
       <c r="M118" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="N118" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="R118" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="T118" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="V118" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Z118" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="AB118" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="120" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R120" t="s">
-        <v>175</v>
-      </c>
-      <c r="T120" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="U120" s="22"/>
+        <v>172</v>
+      </c>
+      <c r="T120" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="U120" s="23"/>
     </row>
     <row r="121" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="122" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="S122" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cập nhật thiết kế màn hình
</commit_message>
<xml_diff>
--- a/api_function_list.xlsx
+++ b/api_function_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="api functions" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="282">
   <si>
     <t>NO.</t>
   </si>
@@ -86,45 +86,12 @@
     <t>Quét QR code</t>
   </si>
   <si>
-    <t>Quét QR code -&gt; chọn món</t>
-  </si>
-  <si>
     <t>Customer scan QR code -&gt; get menu</t>
   </si>
   <si>
-    <t>api/store/&lt;int: id&gt;/menu</t>
-  </si>
-  <si>
-    <t>Chọn món -&gt; order</t>
-  </si>
-  <si>
-    <t>Customer order</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
-    <t>api/store/&lt;int: id&gt;/send-order</t>
-  </si>
-  <si>
-    <t>Quét QR code -&gt; Gửi yêu cầu</t>
-  </si>
-  <si>
-    <t>Customer scan QR code -&gt; send request</t>
-  </si>
-  <si>
-    <t>api/store/&lt;int:id&gt;/send-request</t>
-  </si>
-  <si>
-    <t>Home: customer</t>
-  </si>
-  <si>
-    <t>Load detail home page when user is customer</t>
-  </si>
-  <si>
-    <t>api/customer/&lt;int:id&gt;</t>
-  </si>
-  <si>
     <t>Số điện thoại</t>
   </si>
   <si>
@@ -134,16 +101,7 @@
     <t>Số điện thoại:</t>
   </si>
   <si>
-    <t>Bạn là:</t>
-  </si>
-  <si>
     <t>logo (image)</t>
-  </si>
-  <si>
-    <t>Khách hàng</t>
-  </si>
-  <si>
-    <t>Nhân viên</t>
   </si>
   <si>
     <t>Đăng ký tài khoản</t>
@@ -636,12 +594,300 @@
   <si>
     <t>api/staff/active-pass</t>
   </si>
+  <si>
+    <t>Tách màn hình này giữa customer và staff</t>
+  </si>
+  <si>
+    <t>show camera quét QR code -&gt; màn hình chọn món hoặc gửi yêu cầu</t>
+  </si>
+  <si>
+    <t>Chọn món</t>
+  </si>
+  <si>
+    <t>Gửi yêu cầu</t>
+  </si>
+  <si>
+    <t>Chào mừng bạn đến nhà hàng ABC</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>bàn số:</t>
+  </si>
+  <si>
+    <t>selected box</t>
+  </si>
+  <si>
+    <t>đặt món</t>
+  </si>
+  <si>
+    <t xml:space="preserve">popup: </t>
+  </si>
+  <si>
+    <t>đặt món thành công</t>
+  </si>
+  <si>
+    <t>Đăng ký tài khoản để tích điểm và nhận nhiều khuyến mãi từ nhà hàng</t>
+  </si>
+  <si>
+    <t>(Show dòng trên nếu chưa đăng nhập)</t>
+  </si>
+  <si>
+    <t>Yêu cầu của bạn sẽ được gửi tới nhân viên nhà hàng</t>
+  </si>
+  <si>
+    <t>Gửi</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Show quảng cáo theo customer</t>
+  </si>
+  <si>
+    <t>api/customer/&lt;int:id&gt;/adv</t>
+  </si>
+  <si>
+    <t>Get danh sách điểm theo nhà hàng</t>
+  </si>
+  <si>
+    <t>api/customer/&lt;int:id&gt;/point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer </t>
+  </si>
+  <si>
+    <t>Get chi tiết điễm theo nhà hàng</t>
+  </si>
+  <si>
+    <t>api/point/&lt;int:id&gt;/detail</t>
+  </si>
+  <si>
+    <t>Get danh sách khuyến mãi của nhà hàng</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int:id&gt;/promotion</t>
+  </si>
+  <si>
+    <t>Get danh sách bàn theo nhà hàng</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int:id&gt;/table</t>
+  </si>
+  <si>
+    <t>Đổi điểm</t>
+  </si>
+  <si>
+    <t>api/customer/&lt;int:id&gt;/trade</t>
+  </si>
+  <si>
+    <t>Đặt món</t>
+  </si>
+  <si>
+    <t>api/customer/&lt;int:id&gt;/order</t>
+  </si>
+  <si>
+    <t>api/customer/&lt;int:id&gt;/send-request</t>
+  </si>
+  <si>
+    <t>avatar</t>
+  </si>
+  <si>
+    <t>tên</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>api/staff/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>Staff admin</t>
+  </si>
+  <si>
+    <t>Get danh sách menu</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int: id&gt;/menu-cus</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int:id&gt;/menu-staff</t>
+  </si>
+  <si>
+    <t>Get menu detail</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int:id&gt;/menu/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>Add menu</t>
+  </si>
+  <si>
+    <t>api/menu/add</t>
+  </si>
+  <si>
+    <t>Update menu</t>
+  </si>
+  <si>
+    <t>api/menu/update</t>
+  </si>
+  <si>
+    <t>Delete menu</t>
+  </si>
+  <si>
+    <t>api/menu/delete/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>Get danh sách staff</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int:id&gt;/staff</t>
+  </si>
+  <si>
+    <t>Get staff detail</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int:id&gt;/staff/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>Add staff</t>
+  </si>
+  <si>
+    <t>Update staff</t>
+  </si>
+  <si>
+    <t>api/staff/update</t>
+  </si>
+  <si>
+    <t>Delete staff</t>
+  </si>
+  <si>
+    <t>api/staff/delete/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>chỉ nhân viên của nhà hàng đó mới dc xoá</t>
+  </si>
+  <si>
+    <t>Get danh sách promotion</t>
+  </si>
+  <si>
+    <t>Get promotion detail</t>
+  </si>
+  <si>
+    <t>Add promotion</t>
+  </si>
+  <si>
+    <t>Update promotion</t>
+  </si>
+  <si>
+    <t>Delete promotion</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int:id&gt;/promotion/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>api/promotion/add</t>
+  </si>
+  <si>
+    <t>api/promotion/update</t>
+  </si>
+  <si>
+    <t>api/promotion/delete/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>Get system config</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int:id&gt;/config</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int:id&gt;/config/update</t>
+  </si>
+  <si>
+    <t>Supper admin</t>
+  </si>
+  <si>
+    <t>Update system config</t>
+  </si>
+  <si>
+    <t>Get danh sách store</t>
+  </si>
+  <si>
+    <t>Get store detail</t>
+  </si>
+  <si>
+    <t>Add store</t>
+  </si>
+  <si>
+    <t>Update store</t>
+  </si>
+  <si>
+    <t>Delete store</t>
+  </si>
+  <si>
+    <t>api/store/list</t>
+  </si>
+  <si>
+    <t>api/store/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>api/store/add</t>
+  </si>
+  <si>
+    <t>api/store/update</t>
+  </si>
+  <si>
+    <t>api/store/delete/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>Xoá store thì xoá hết nhân viên thuộc nhà hàng đó</t>
+  </si>
+  <si>
+    <t>Get danh sách store admin</t>
+  </si>
+  <si>
+    <t>api/store-admin/list</t>
+  </si>
+  <si>
+    <t>api/store-admin/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>api/store-admin/add</t>
+  </si>
+  <si>
+    <t>api/store-admin/update</t>
+  </si>
+  <si>
+    <t>api/store-admin/delete/&lt;int:id&gt;</t>
+  </si>
+  <si>
+    <t>Get store admin detail</t>
+  </si>
+  <si>
+    <t>Add store admin</t>
+  </si>
+  <si>
+    <t>Update store admin</t>
+  </si>
+  <si>
+    <t>Delete store admin</t>
+  </si>
+  <si>
+    <t>nhân viên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">màn hình đăng nhập của </t>
+  </si>
+  <si>
+    <t>nhân viên: bỏ đăng ký va quét QR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -680,6 +926,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -689,7 +942,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -818,11 +1071,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -837,6 +1185,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -865,12 +1219,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -888,6 +1236,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1193,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G16"/>
+  <dimension ref="A2:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1588,7 @@
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1226,7 +1610,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>4</v>
@@ -1249,10 +1633,10 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="G3" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1272,10 +1656,10 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1295,10 +1679,10 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1318,10 +1702,10 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1329,7 +1713,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1338,13 +1722,13 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="F7" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1352,7 +1736,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -1361,18 +1745,21 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -1381,109 +1768,688 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="F9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" t="s">
         <v>184</v>
-      </c>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>197</v>
-      </c>
-      <c r="C10" t="s">
-        <v>198</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="F10" t="s">
-        <v>184</v>
-      </c>
-      <c r="G10" s="12"/>
+        <v>170</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>201</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>204</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>206</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>207</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>201</v>
+      </c>
+      <c r="C18" t="s">
+        <v>215</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C19" t="s">
+        <v>189</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
+        <v>220</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C21" t="s">
+        <v>223</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>222</v>
+      </c>
+      <c r="C23" t="s">
+        <v>228</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" t="s">
+        <v>230</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>222</v>
+      </c>
+      <c r="C25" t="s">
+        <v>232</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>233</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>222</v>
+      </c>
+      <c r="C26" t="s">
+        <v>234</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C27" t="s">
+        <v>236</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>222</v>
+      </c>
+      <c r="C28" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>171</v>
+      </c>
+      <c r="F28" t="s">
+        <v>170</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" t="s">
+        <v>239</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" t="s">
+        <v>241</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>242</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C31" t="s">
+        <v>244</v>
+      </c>
+      <c r="D31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32" t="s">
+        <v>245</v>
+      </c>
+      <c r="D32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>222</v>
+      </c>
+      <c r="C33" t="s">
+        <v>246</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>250</v>
+      </c>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" t="s">
+        <v>247</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C35" t="s">
+        <v>248</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>252</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>34</v>
       </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="B36" t="s">
+        <v>222</v>
+      </c>
+      <c r="C36" t="s">
+        <v>253</v>
+      </c>
+      <c r="D36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>185</v>
-      </c>
-      <c r="F16" t="s">
-        <v>184</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>186</v>
-      </c>
+      <c r="B37" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37" t="s">
+        <v>257</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>256</v>
+      </c>
+      <c r="C38" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>256</v>
+      </c>
+      <c r="C39" t="s">
+        <v>259</v>
+      </c>
+      <c r="D39" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>256</v>
+      </c>
+      <c r="C40" t="s">
+        <v>260</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>265</v>
+      </c>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>256</v>
+      </c>
+      <c r="C41" t="s">
+        <v>261</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>256</v>
+      </c>
+      <c r="C42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>267</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>256</v>
+      </c>
+      <c r="C43" t="s">
+        <v>269</v>
+      </c>
+      <c r="D43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>256</v>
+      </c>
+      <c r="C44" t="s">
+        <v>275</v>
+      </c>
+      <c r="D44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>256</v>
+      </c>
+      <c r="C45" t="s">
+        <v>276</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>272</v>
+      </c>
+      <c r="G45" s="12"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>256</v>
+      </c>
+      <c r="C46" t="s">
+        <v>277</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>256</v>
+      </c>
+      <c r="C47" t="s">
+        <v>278</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>274</v>
+      </c>
+      <c r="G47" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1493,10 +2459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AJ122"/>
+  <dimension ref="B2:AN122"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,137 +2473,149 @@
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C2" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" s="42" t="s">
+        <v>279</v>
+      </c>
       <c r="N2" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:36" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="43" t="s">
+        <v>280</v>
+      </c>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+    </row>
     <row r="5" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" t="s">
         <v>38</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="T5" t="s">
-        <v>52</v>
       </c>
       <c r="U5" s="3"/>
       <c r="W5" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="Y5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" t="s">
         <v>38</v>
-      </c>
-      <c r="AB5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>52</v>
       </c>
       <c r="AH5" s="3"/>
       <c r="AJ5" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
       <c r="U6" s="5" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="AH6" s="5" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="M7" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="Y7" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="M9" t="s">
+        <v>31</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q9" s="14"/>
+      <c r="Y9" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" t="s">
-        <v>45</v>
-      </c>
-      <c r="P9" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q9" s="23"/>
-      <c r="Y9" t="s">
-        <v>55</v>
-      </c>
       <c r="AB9" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AB10" s="5" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1645,32 +2623,32 @@
         <v>14</v>
       </c>
       <c r="M11" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="P11" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z11" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA11" s="23"/>
+        <v>48</v>
+      </c>
+      <c r="Z11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA11" s="14"/>
     </row>
     <row r="12" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P12" s="5" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="M13" t="s">
-        <v>48</v>
-      </c>
-      <c r="P13" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q13" s="23"/>
+        <v>34</v>
+      </c>
+      <c r="P13" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q13" s="14"/>
     </row>
     <row r="14" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="2" t="s">
@@ -1682,119 +2660,155 @@
         <v>22</v>
       </c>
       <c r="M15" t="s">
-        <v>49</v>
-      </c>
-      <c r="P15" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q15" s="23"/>
+        <v>35</v>
+      </c>
+      <c r="P15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q15" s="14"/>
     </row>
     <row r="16" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="M17" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M19" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P20" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O21" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>76</v>
+        <v>62</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="V23" s="1"/>
-    </row>
-    <row r="24" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC23" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ23" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G24" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="H24" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B25" s="24" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C25" s="25"/>
       <c r="E25" s="24" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="F25" s="25"/>
       <c r="H25" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="L25" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="N25">
         <v>300000</v>
       </c>
-    </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V25" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>191</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B26" s="26"/>
       <c r="C26" s="27"/>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="27"/>
       <c r="H26" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI26" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="26"/>
       <c r="C27" s="27"/>
       <c r="E27" s="26"/>
       <c r="F27" s="27"/>
       <c r="H27" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="L27" t="s">
+        <v>57</v>
+      </c>
+      <c r="M27" t="s">
+        <v>70</v>
+      </c>
+      <c r="O27" t="s">
         <v>71</v>
       </c>
-      <c r="M27" t="s">
-        <v>84</v>
-      </c>
-      <c r="O27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AL27" s="35"/>
+      <c r="AM27" s="36"/>
+      <c r="AN27" s="37"/>
+    </row>
+    <row r="28" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
       <c r="E28" s="28"/>
@@ -1803,66 +2817,98 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="O28">
         <v>3000</v>
       </c>
       <c r="Q28" s="8" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="R28" s="8" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="S28" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V28" t="s">
+        <v>190</v>
+      </c>
+      <c r="AL28" s="33"/>
+      <c r="AM28" s="19"/>
+      <c r="AN28" s="38"/>
+    </row>
+    <row r="29" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L29">
         <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="O29">
         <v>4000</v>
       </c>
       <c r="Q29" s="8" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="R29" s="8" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="S29" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="22" t="s">
+      <c r="AL29" s="39"/>
+      <c r="AM29" s="40"/>
+      <c r="AN29" s="41"/>
+    </row>
+    <row r="30" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="23"/>
-    </row>
-    <row r="31" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="14"/>
+      <c r="V30" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="W30" s="32"/>
+    </row>
+    <row r="31" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>192</v>
+      </c>
+      <c r="AE31" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="AF31" s="32"/>
+      <c r="AM31" s="31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="V32" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="W32" s="32"/>
+    </row>
+    <row r="33" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AE33" s="31" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
@@ -1874,65 +2920,79 @@
       <c r="K34" s="11"/>
       <c r="L34" s="11"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E35" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E36">
         <v>55000</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I36" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="J36" s="23"/>
-    </row>
-    <row r="37" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J36" s="14"/>
+      <c r="AC36" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E37">
         <v>30000</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I37" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="J37" s="23"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J37" s="14"/>
+      <c r="AD37" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="2:31" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="F39" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="G39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="2:31" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>1</v>
       </c>
@@ -1943,7 +3003,7 @@
         <v>43821</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
       <c r="E41">
         <v>2</v>
       </c>
@@ -1954,125 +3014,138 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I48" t="s">
+        <v>219</v>
+      </c>
+      <c r="J48" t="s">
+        <v>218</v>
+      </c>
+    </row>
     <row r="49" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C49" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="15"/>
+      <c r="C49" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="17"/>
+      <c r="J49" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="50" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C50" s="16"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="20"/>
+      <c r="J50" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="51" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C51" s="16"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="20"/>
     </row>
     <row r="52" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="19"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="23"/>
     </row>
     <row r="55" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="23"/>
+      <c r="C57" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="14"/>
       <c r="G57" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="T57" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K58" s="3" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D59" s="23"/>
+      <c r="C59" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D59" s="14"/>
       <c r="U59" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N60" t="s">
+        <v>30</v>
+      </c>
+      <c r="P60" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P60" s="3" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="61" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="14"/>
+      <c r="F61" t="s">
+        <v>57</v>
+      </c>
+      <c r="G61" t="s">
+        <v>87</v>
+      </c>
+      <c r="H61" t="s">
+        <v>88</v>
+      </c>
+      <c r="I61" t="s">
+        <v>89</v>
+      </c>
+      <c r="P61" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="D61" s="23"/>
-      <c r="F61" t="s">
-        <v>71</v>
-      </c>
-      <c r="G61" t="s">
-        <v>101</v>
-      </c>
-      <c r="H61" t="s">
-        <v>102</v>
-      </c>
-      <c r="I61" t="s">
-        <v>103</v>
-      </c>
-      <c r="P61" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="Q61" s="5"/>
       <c r="V61" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2080,129 +3153,129 @@
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="H62">
         <v>30000</v>
       </c>
       <c r="I62" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="K62" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="L62" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="N62" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C63" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D63" s="23"/>
+      <c r="C63" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63" s="14"/>
       <c r="F63">
         <v>2</v>
       </c>
       <c r="G63" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="H63">
         <v>20000</v>
       </c>
       <c r="I63" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="K63" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="L63" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="P63" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="V63" s="3" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="X63" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N64" t="s">
-        <v>111</v>
-      </c>
-      <c r="P64" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q64" s="23"/>
+        <v>97</v>
+      </c>
+      <c r="P64" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q64" s="14"/>
       <c r="R64" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R65" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P66" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="6:25" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G71" s="1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="U71" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K72" s="3" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P73" t="s">
+        <v>30</v>
+      </c>
+      <c r="R73" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R73" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="V73" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F74" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G74" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="H74" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J74" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="K74" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="R74" s="5"/>
       <c r="S74" s="5"/>
@@ -2212,104 +3285,104 @@
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="J75" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="K75" s="7">
         <v>43821</v>
       </c>
       <c r="M75" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="N75" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="P75" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="R75" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="W75" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R76" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P77" t="s">
-        <v>122</v>
-      </c>
-      <c r="R77" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="S77" s="23"/>
+        <v>108</v>
+      </c>
+      <c r="R77" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="S77" s="14"/>
       <c r="W77" s="3" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="Y77" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="78" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="79" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q79" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="81" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G81" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="P81" s="1" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="U81" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K82" s="3" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P83" t="s">
+        <v>30</v>
+      </c>
+      <c r="R83" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R83" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="V83" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F84" t="s">
+        <v>57</v>
+      </c>
+      <c r="G84" t="s">
+        <v>87</v>
+      </c>
+      <c r="H84" t="s">
         <v>71</v>
       </c>
-      <c r="G84" t="s">
-        <v>101</v>
-      </c>
-      <c r="H84" t="s">
-        <v>85</v>
-      </c>
       <c r="I84" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="K84" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="R84" s="5" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="S84" s="5"/>
     </row>
@@ -2318,7 +3391,7 @@
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="H85">
         <v>1000</v>
@@ -2330,170 +3403,170 @@
         <v>43730</v>
       </c>
       <c r="M85" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="N85" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="P85" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="R85" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="W85" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R86" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P87" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="R87" s="10" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="T87" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="W87" s="3" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="Y87" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="88" spans="2:25" x14ac:dyDescent="0.25">
       <c r="R88" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="90" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G90" s="1" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="Q90" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="91" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K91" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="92" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="93" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G93" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="K93" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="G96" s="9"/>
     </row>
     <row r="97" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="98" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C98" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="D98" s="23"/>
+      <c r="C98" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D98" s="14"/>
       <c r="F98" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="N98" s="3" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="R98" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="X98" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C100" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="D100" s="23"/>
+      <c r="C100" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D100" s="14"/>
       <c r="F100" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="I100" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="K100" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="M100" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="N100" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="R100" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="T100" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="Y100" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="101" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="102" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N102" s="3" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="R102" t="s">
-        <v>48</v>
-      </c>
-      <c r="T102" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="U102" s="23"/>
+        <v>34</v>
+      </c>
+      <c r="T102" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="U102" s="14"/>
       <c r="Z102" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="103" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F103" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G103" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="H103" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="J103" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="K103" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="L103" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="N103" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2501,16 +3574,16 @@
         <v>1</v>
       </c>
       <c r="G104" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="H104" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="J104" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="K104" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L104" s="7">
         <v>44187</v>
@@ -2519,130 +3592,130 @@
         <v>43821</v>
       </c>
       <c r="P104" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="Q104" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="R104" t="s">
-        <v>49</v>
-      </c>
-      <c r="T104" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="U104" s="23"/>
+        <v>35</v>
+      </c>
+      <c r="T104" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="U104" s="14"/>
       <c r="Z104" s="3" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="AB104" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="106" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R106" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="T106" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="X106" s="5" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="108" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R108" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="T108" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="V108" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="109" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="110" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T110" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="111" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="112" spans="3:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F112" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="O112" s="3" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="R112" s="1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="X112" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="113" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="114" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F114" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="I114" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="M114" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="O114" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="R114" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="T114" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="Y114" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="115" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="116" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O116" s="3" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="R116" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="T116" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="Z116" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="117" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F117" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G117" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="H117" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J117" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="K117" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="118" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2650,57 +3723,74 @@
         <v>1</v>
       </c>
       <c r="G118" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="H118" s="8" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="J118" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="K118" s="7">
         <v>43821</v>
       </c>
       <c r="M118" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="N118" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="R118" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="T118" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="V118" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="Z118" s="3" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="AB118" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="119" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="120" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R120" t="s">
-        <v>172</v>
-      </c>
-      <c r="T120" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="U120" s="23"/>
+        <v>158</v>
+      </c>
+      <c r="T120" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="U120" s="14"/>
     </row>
     <row r="121" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="122" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="S122" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="28">
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="AL27:AN29"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="C49:H52"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="Z11:AA11"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="B25:C28"/>
+    <mergeCell ref="E25:F28"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V32:W32"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C61:D61"/>
@@ -2712,16 +3802,6 @@
     <mergeCell ref="C100:D100"/>
     <mergeCell ref="T102:U102"/>
     <mergeCell ref="T104:U104"/>
-    <mergeCell ref="C49:H52"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="Z11:AA11"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="B25:C28"/>
-    <mergeCell ref="E25:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add api get pmt by cus
</commit_message>
<xml_diff>
--- a/api_function_list.xlsx
+++ b/api_function_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="755" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="755" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="screens" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="413">
   <si>
     <t>NO.</t>
   </si>
@@ -1370,6 +1370,27 @@
   </si>
   <si>
     <t>api/master/city/&lt;int:id&gt;/district</t>
+  </si>
+  <si>
+    <t>Promotion</t>
+  </si>
+  <si>
+    <t>Get danh sách khuyến mãi khả dụng</t>
+  </si>
+  <si>
+    <t>api/customer/pmt/owned</t>
+  </si>
+  <si>
+    <t>Get danh sách khuyến mãi đã dùng</t>
+  </si>
+  <si>
+    <t>api/customer/pmt/used</t>
+  </si>
+  <si>
+    <t>Get danh sách khuyến mãi đã hết hạn</t>
+  </si>
+  <si>
+    <t>api/customer/pmt/expired</t>
   </si>
 </sst>
 </file>
@@ -5402,10 +5423,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G11"/>
+  <dimension ref="A2:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5613,6 +5634,66 @@
         <v>370</v>
       </c>
       <c r="F11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>406</v>
+      </c>
+      <c r="C12" t="s">
+        <v>407</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>408</v>
+      </c>
+      <c r="F12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>406</v>
+      </c>
+      <c r="C13" t="s">
+        <v>409</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>410</v>
+      </c>
+      <c r="F13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>406</v>
+      </c>
+      <c r="C14" t="s">
+        <v>411</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>412</v>
+      </c>
+      <c r="F14" t="s">
         <v>136</v>
       </c>
     </row>
@@ -6412,7 +6493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -6548,7 +6629,7 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add api: get list store
</commit_message>
<xml_diff>
--- a/api_function_list.xlsx
+++ b/api_function_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="755" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="755" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="screens" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="416">
   <si>
     <t>NO.</t>
   </si>
@@ -1391,6 +1391,15 @@
   </si>
   <si>
     <t>api/customer/pmt/expired</t>
+  </si>
+  <si>
+    <t>Admin store</t>
+  </si>
+  <si>
+    <t>Get list store</t>
+  </si>
+  <si>
+    <t>api/store/list</t>
   </si>
 </sst>
 </file>
@@ -1806,10 +1815,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1830,9 +1872,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1843,9 +1882,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1869,34 +1905,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2355,15 +2364,15 @@
     </row>
     <row r="5" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="19"/>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="49"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="49"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="8" t="s">
         <v>218</v>
       </c>
@@ -2413,13 +2422,13 @@
     </row>
     <row r="6" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="19"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="50"/>
-      <c r="F6" s="51"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="62"/>
       <c r="G6" s="8" t="s">
         <v>219</v>
       </c>
@@ -2459,11 +2468,11 @@
     </row>
     <row r="7" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="19"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="51"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8" t="s">
@@ -2494,11 +2503,11 @@
     </row>
     <row r="8" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="19"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="64"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -2536,11 +2545,11 @@
         <v>327</v>
       </c>
       <c r="M9" s="8"/>
-      <c r="N9" s="46" t="s">
+      <c r="N9" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="O9" s="54"/>
-      <c r="P9" s="47"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="57"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="21"/>
       <c r="Z9" s="19" t="s">
@@ -2557,10 +2566,10 @@
     </row>
     <row r="10" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="19"/>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -2609,10 +2618,10 @@
       <c r="Q11" s="8"/>
       <c r="R11" s="21"/>
       <c r="Z11" s="25"/>
-      <c r="AA11" s="46" t="s">
+      <c r="AA11" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="AB11" s="47"/>
+      <c r="AB11" s="57"/>
       <c r="AC11" s="26"/>
       <c r="AD11" s="26"/>
       <c r="AE11" s="26"/>
@@ -2655,11 +2664,11 @@
         <v>328</v>
       </c>
       <c r="M13" s="8"/>
-      <c r="N13" s="46" t="s">
+      <c r="N13" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="O13" s="54"/>
-      <c r="P13" s="47"/>
+      <c r="O13" s="76"/>
+      <c r="P13" s="57"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="21"/>
     </row>
@@ -2709,11 +2718,11 @@
         <v>329</v>
       </c>
       <c r="M15" s="8"/>
-      <c r="N15" s="46" t="s">
+      <c r="N15" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="54"/>
-      <c r="P15" s="47"/>
+      <c r="O15" s="76"/>
+      <c r="P15" s="57"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="21"/>
     </row>
@@ -3148,11 +3157,11 @@
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="21"/>
-      <c r="H27" s="64" t="s">
+      <c r="H27" s="73" t="s">
         <v>213</v>
       </c>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
       <c r="L27" s="19" t="s">
         <v>229</v>
       </c>
@@ -3181,9 +3190,9 @@
       <c r="AI27" s="21"/>
       <c r="AJ27" s="19"/>
       <c r="AK27" s="8"/>
-      <c r="AL27" s="68"/>
-      <c r="AM27" s="69"/>
-      <c r="AN27" s="70"/>
+      <c r="AL27" s="47"/>
+      <c r="AM27" s="48"/>
+      <c r="AN27" s="49"/>
       <c r="AO27" s="21"/>
       <c r="AQ27" s="19">
         <v>1</v>
@@ -3228,11 +3237,11 @@
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="21"/>
-      <c r="H28" s="61" t="s">
+      <c r="H28" s="70" t="s">
         <v>355</v>
       </c>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
       <c r="L28" s="19"/>
       <c r="M28" s="8"/>
       <c r="N28" s="21"/>
@@ -3261,9 +3270,9 @@
       <c r="AI28" s="21"/>
       <c r="AJ28" s="19"/>
       <c r="AK28" s="8"/>
-      <c r="AL28" s="71"/>
-      <c r="AM28" s="59"/>
-      <c r="AN28" s="72"/>
+      <c r="AL28" s="50"/>
+      <c r="AM28" s="51"/>
+      <c r="AN28" s="52"/>
       <c r="AO28" s="21"/>
       <c r="AQ28" s="19">
         <v>2</v>
@@ -3302,9 +3311,9 @@
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="21"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="66"/>
-      <c r="J29" s="66"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75"/>
       <c r="L29" s="19" t="s">
         <v>230</v>
       </c>
@@ -3326,9 +3335,9 @@
       <c r="AI29" s="21"/>
       <c r="AJ29" s="19"/>
       <c r="AK29" s="8"/>
-      <c r="AL29" s="73"/>
-      <c r="AM29" s="74"/>
-      <c r="AN29" s="75"/>
+      <c r="AL29" s="53"/>
+      <c r="AM29" s="54"/>
+      <c r="AN29" s="55"/>
       <c r="AO29" s="21"/>
       <c r="AQ29" s="19"/>
       <c r="AR29" s="8"/>
@@ -3365,10 +3374,10 @@
       <c r="R30" s="7"/>
       <c r="S30" s="7"/>
       <c r="U30" s="19"/>
-      <c r="V30" s="67" t="s">
+      <c r="V30" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="W30" s="67"/>
+      <c r="W30" s="46"/>
       <c r="X30" s="8"/>
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
@@ -3436,10 +3445,10 @@
       <c r="AD31" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="AE31" s="67" t="s">
+      <c r="AE31" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="AF31" s="67"/>
+      <c r="AF31" s="46"/>
       <c r="AG31" s="8"/>
       <c r="AH31" s="8"/>
       <c r="AI31" s="21"/>
@@ -3482,10 +3491,10 @@
       <c r="E32" s="8"/>
       <c r="F32" s="21"/>
       <c r="U32" s="25"/>
-      <c r="V32" s="76" t="s">
+      <c r="V32" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="W32" s="76"/>
+      <c r="W32" s="58"/>
       <c r="X32" s="26"/>
       <c r="Y32" s="26"/>
       <c r="Z32" s="26"/>
@@ -3703,14 +3712,14 @@
     <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A49" s="19"/>
       <c r="B49" s="8"/>
-      <c r="C49" s="55" t="s">
+      <c r="C49" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="57"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="67"/>
       <c r="I49" s="8"/>
       <c r="J49" s="8" t="s">
         <v>132</v>
@@ -3725,12 +3734,12 @@
     <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A50" s="19"/>
       <c r="B50" s="8"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="60"/>
+      <c r="C50" s="68"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="69"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8" t="s">
         <v>133</v>
@@ -3743,12 +3752,12 @@
     <row r="51" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="19"/>
       <c r="B51" s="8"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="60"/>
+      <c r="C51" s="68"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="69"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
       <c r="K51" s="21"/>
@@ -3759,12 +3768,12 @@
     <row r="52" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="19"/>
       <c r="B52" s="8"/>
-      <c r="C52" s="61"/>
-      <c r="D52" s="62"/>
-      <c r="E52" s="62"/>
-      <c r="F52" s="62"/>
-      <c r="G52" s="62"/>
-      <c r="H52" s="63"/>
+      <c r="C52" s="70"/>
+      <c r="D52" s="71"/>
+      <c r="E52" s="71"/>
+      <c r="F52" s="71"/>
+      <c r="G52" s="71"/>
+      <c r="H52" s="72"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
       <c r="K52" s="21"/>
@@ -3789,10 +3798,10 @@
     </row>
     <row r="56" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="57" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C57" s="46" t="s">
+      <c r="C57" s="56" t="s">
         <v>375</v>
       </c>
-      <c r="D57" s="47"/>
+      <c r="D57" s="57"/>
       <c r="F57" s="1" t="s">
         <v>376</v>
       </c>
@@ -3812,10 +3821,10 @@
       </c>
     </row>
     <row r="59" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C59" s="46" t="s">
+      <c r="C59" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="D59" s="47"/>
+      <c r="D59" s="57"/>
       <c r="F59" t="s">
         <v>44</v>
       </c>
@@ -3859,10 +3868,10 @@
       </c>
     </row>
     <row r="61" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C61" s="46" t="s">
+      <c r="C61" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="D61" s="47"/>
+      <c r="D61" s="57"/>
       <c r="O61" s="4" t="s">
         <v>74</v>
       </c>
@@ -3880,10 +3889,10 @@
       </c>
     </row>
     <row r="63" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C63" s="46" t="s">
+      <c r="C63" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="D63" s="47"/>
+      <c r="D63" s="57"/>
       <c r="O63" s="5" t="s">
         <v>75</v>
       </c>
@@ -3898,19 +3907,19 @@
       <c r="M64" t="s">
         <v>336</v>
       </c>
-      <c r="O64" s="46" t="s">
+      <c r="O64" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="P64" s="47"/>
+      <c r="P64" s="57"/>
       <c r="Q64" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="65" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C65" s="46" t="s">
+      <c r="C65" s="56" t="s">
         <v>296</v>
       </c>
-      <c r="D65" s="47"/>
+      <c r="D65" s="57"/>
       <c r="Q65" t="s">
         <v>77</v>
       </c>
@@ -3921,10 +3930,10 @@
       </c>
     </row>
     <row r="67" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C67" s="46" t="s">
+      <c r="C67" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="D67" s="47"/>
+      <c r="D67" s="57"/>
       <c r="F67" s="15"/>
       <c r="G67" s="17"/>
       <c r="H67" s="17"/>
@@ -3955,10 +3964,10 @@
       </c>
     </row>
     <row r="69" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C69" s="46" t="s">
+      <c r="C69" s="56" t="s">
         <v>312</v>
       </c>
-      <c r="D69" s="47"/>
+      <c r="D69" s="57"/>
       <c r="F69" s="19"/>
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
@@ -4116,10 +4125,10 @@
       <c r="P75" t="s">
         <v>379</v>
       </c>
-      <c r="R75" s="46" t="s">
+      <c r="R75" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="S75" s="47"/>
+      <c r="S75" s="57"/>
       <c r="T75" t="s">
         <v>380</v>
       </c>
@@ -4140,10 +4149,10 @@
       <c r="P77" t="s">
         <v>336</v>
       </c>
-      <c r="R77" s="46" t="s">
+      <c r="R77" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="S77" s="47"/>
+      <c r="S77" s="57"/>
       <c r="T77" t="s">
         <v>381</v>
       </c>
@@ -4575,10 +4584,10 @@
     </row>
     <row r="125" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="126" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C126" s="46" t="s">
+      <c r="C126" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="D126" s="47"/>
+      <c r="D126" s="57"/>
       <c r="F126" t="s">
         <v>28</v>
       </c>
@@ -4609,10 +4618,10 @@
     </row>
     <row r="127" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="128" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C128" s="46" t="s">
+      <c r="C128" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="D128" s="47"/>
+      <c r="D128" s="57"/>
       <c r="N128" s="2" t="s">
         <v>108</v>
       </c>
@@ -4948,10 +4957,10 @@
       <c r="E160" s="19"/>
       <c r="F160" s="8"/>
       <c r="G160" s="8"/>
-      <c r="H160" s="48" t="s">
+      <c r="H160" s="59" t="s">
         <v>390</v>
       </c>
-      <c r="I160" s="49"/>
+      <c r="I160" s="60"/>
       <c r="J160" s="8"/>
       <c r="K160" s="21"/>
     </row>
@@ -4959,8 +4968,8 @@
       <c r="E161" s="19"/>
       <c r="F161" s="8"/>
       <c r="G161" s="8"/>
-      <c r="H161" s="50"/>
-      <c r="I161" s="51"/>
+      <c r="H161" s="61"/>
+      <c r="I161" s="62"/>
       <c r="J161" s="8"/>
       <c r="K161" s="21"/>
     </row>
@@ -4968,8 +4977,8 @@
       <c r="E162" s="19"/>
       <c r="F162" s="8"/>
       <c r="G162" s="8"/>
-      <c r="H162" s="50"/>
-      <c r="I162" s="51"/>
+      <c r="H162" s="61"/>
+      <c r="I162" s="62"/>
       <c r="J162" s="8"/>
       <c r="K162" s="21"/>
     </row>
@@ -4977,8 +4986,8 @@
       <c r="E163" s="19"/>
       <c r="F163" s="8"/>
       <c r="G163" s="8"/>
-      <c r="H163" s="50"/>
-      <c r="I163" s="51"/>
+      <c r="H163" s="61"/>
+      <c r="I163" s="62"/>
       <c r="J163" s="8"/>
       <c r="K163" s="21"/>
     </row>
@@ -4986,8 +4995,8 @@
       <c r="E164" s="19"/>
       <c r="F164" s="8"/>
       <c r="G164" s="8"/>
-      <c r="H164" s="52"/>
-      <c r="I164" s="53"/>
+      <c r="H164" s="63"/>
+      <c r="I164" s="64"/>
       <c r="J164" s="8"/>
       <c r="K164" s="21"/>
     </row>
@@ -5108,23 +5117,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="AL27:AN29"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="B5:C8"/>
-    <mergeCell ref="E5:F8"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C49:H52"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H29:J29"/>
     <mergeCell ref="R75:S75"/>
     <mergeCell ref="R77:S77"/>
     <mergeCell ref="H160:I164"/>
@@ -5136,6 +5128,23 @@
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="O64:P64"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B5:C8"/>
+    <mergeCell ref="E5:F8"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C49:H52"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="AL27:AN29"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="V32:W32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6224,10 +6233,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G12"/>
+  <dimension ref="A2:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6483,6 +6492,26 @@
         <v>136</v>
       </c>
       <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>413</v>
+      </c>
+      <c r="C13" t="s">
+        <v>414</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>415</v>
+      </c>
+      <c r="F13" t="s">
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6628,7 +6657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add api: update customer info
</commit_message>
<xml_diff>
--- a/api_function_list.xlsx
+++ b/api_function_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="755" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="screens" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="419">
   <si>
     <t>NO.</t>
   </si>
@@ -1400,6 +1400,22 @@
   </si>
   <si>
     <t>api/store/list</t>
+  </si>
+  <si>
+    <t>Cập nhật thông tin cá nhân</t>
+  </si>
+  <si>
+    <t>api/customer/update-info</t>
+  </si>
+  <si>
+    <t>{
+"name": "test update",
+"phone_number": "0976111444",
+"gender": 1,
+"birthday": "1992-12-23",
+"city_id": 1, 
+"district_id": 2
+}</t>
   </si>
 </sst>
 </file>
@@ -1815,43 +1831,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1872,6 +1855,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1882,6 +1868,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1905,7 +1894,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2214,7 +2230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG175"/>
   <sheetViews>
-    <sheetView topLeftCell="L82" workbookViewId="0">
+    <sheetView topLeftCell="J25" workbookViewId="0">
       <selection activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
@@ -2364,15 +2380,15 @@
     </row>
     <row r="5" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="19"/>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="60"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="8" t="s">
         <v>218</v>
       </c>
@@ -2422,13 +2438,13 @@
     </row>
     <row r="6" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="19"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="62"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="51"/>
       <c r="G6" s="8" t="s">
         <v>219</v>
       </c>
@@ -2468,11 +2484,11 @@
     </row>
     <row r="7" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="19"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="62"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="62"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="51"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8" t="s">
@@ -2503,11 +2519,11 @@
     </row>
     <row r="8" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="19"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="64"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="64"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="53"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -2545,11 +2561,11 @@
         <v>327</v>
       </c>
       <c r="M9" s="8"/>
-      <c r="N9" s="56" t="s">
+      <c r="N9" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O9" s="76"/>
-      <c r="P9" s="57"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="47"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="21"/>
       <c r="Z9" s="19" t="s">
@@ -2566,10 +2582,10 @@
     </row>
     <row r="10" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="19"/>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="57"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -2618,10 +2634,10 @@
       <c r="Q11" s="8"/>
       <c r="R11" s="21"/>
       <c r="Z11" s="25"/>
-      <c r="AA11" s="56" t="s">
+      <c r="AA11" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="AB11" s="57"/>
+      <c r="AB11" s="47"/>
       <c r="AC11" s="26"/>
       <c r="AD11" s="26"/>
       <c r="AE11" s="26"/>
@@ -2664,11 +2680,11 @@
         <v>328</v>
       </c>
       <c r="M13" s="8"/>
-      <c r="N13" s="56" t="s">
+      <c r="N13" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O13" s="76"/>
-      <c r="P13" s="57"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="47"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="21"/>
     </row>
@@ -2718,11 +2734,11 @@
         <v>329</v>
       </c>
       <c r="M15" s="8"/>
-      <c r="N15" s="56" t="s">
+      <c r="N15" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="76"/>
-      <c r="P15" s="57"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="47"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="21"/>
     </row>
@@ -3157,11 +3173,11 @@
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="21"/>
-      <c r="H27" s="73" t="s">
+      <c r="H27" s="64" t="s">
         <v>213</v>
       </c>
-      <c r="I27" s="74"/>
-      <c r="J27" s="74"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
       <c r="L27" s="19" t="s">
         <v>229</v>
       </c>
@@ -3190,9 +3206,9 @@
       <c r="AI27" s="21"/>
       <c r="AJ27" s="19"/>
       <c r="AK27" s="8"/>
-      <c r="AL27" s="47"/>
-      <c r="AM27" s="48"/>
-      <c r="AN27" s="49"/>
+      <c r="AL27" s="68"/>
+      <c r="AM27" s="69"/>
+      <c r="AN27" s="70"/>
       <c r="AO27" s="21"/>
       <c r="AQ27" s="19">
         <v>1</v>
@@ -3237,11 +3253,11 @@
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="21"/>
-      <c r="H28" s="70" t="s">
+      <c r="H28" s="61" t="s">
         <v>355</v>
       </c>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
       <c r="L28" s="19"/>
       <c r="M28" s="8"/>
       <c r="N28" s="21"/>
@@ -3270,9 +3286,9 @@
       <c r="AI28" s="21"/>
       <c r="AJ28" s="19"/>
       <c r="AK28" s="8"/>
-      <c r="AL28" s="50"/>
-      <c r="AM28" s="51"/>
-      <c r="AN28" s="52"/>
+      <c r="AL28" s="71"/>
+      <c r="AM28" s="59"/>
+      <c r="AN28" s="72"/>
       <c r="AO28" s="21"/>
       <c r="AQ28" s="19">
         <v>2</v>
@@ -3311,9 +3327,9 @@
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="21"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="75"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
+      <c r="J29" s="66"/>
       <c r="L29" s="19" t="s">
         <v>230</v>
       </c>
@@ -3335,9 +3351,9 @@
       <c r="AI29" s="21"/>
       <c r="AJ29" s="19"/>
       <c r="AK29" s="8"/>
-      <c r="AL29" s="53"/>
-      <c r="AM29" s="54"/>
-      <c r="AN29" s="55"/>
+      <c r="AL29" s="73"/>
+      <c r="AM29" s="74"/>
+      <c r="AN29" s="75"/>
       <c r="AO29" s="21"/>
       <c r="AQ29" s="19"/>
       <c r="AR29" s="8"/>
@@ -3374,10 +3390,10 @@
       <c r="R30" s="7"/>
       <c r="S30" s="7"/>
       <c r="U30" s="19"/>
-      <c r="V30" s="46" t="s">
+      <c r="V30" s="67" t="s">
         <v>154</v>
       </c>
-      <c r="W30" s="46"/>
+      <c r="W30" s="67"/>
       <c r="X30" s="8"/>
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
@@ -3445,10 +3461,10 @@
       <c r="AD31" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="AE31" s="46" t="s">
+      <c r="AE31" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="AF31" s="46"/>
+      <c r="AF31" s="67"/>
       <c r="AG31" s="8"/>
       <c r="AH31" s="8"/>
       <c r="AI31" s="21"/>
@@ -3491,10 +3507,10 @@
       <c r="E32" s="8"/>
       <c r="F32" s="21"/>
       <c r="U32" s="25"/>
-      <c r="V32" s="58" t="s">
+      <c r="V32" s="76" t="s">
         <v>155</v>
       </c>
-      <c r="W32" s="58"/>
+      <c r="W32" s="76"/>
       <c r="X32" s="26"/>
       <c r="Y32" s="26"/>
       <c r="Z32" s="26"/>
@@ -3712,14 +3728,14 @@
     <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A49" s="19"/>
       <c r="B49" s="8"/>
-      <c r="C49" s="65" t="s">
+      <c r="C49" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="66"/>
-      <c r="E49" s="66"/>
-      <c r="F49" s="66"/>
-      <c r="G49" s="66"/>
-      <c r="H49" s="67"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="57"/>
       <c r="I49" s="8"/>
       <c r="J49" s="8" t="s">
         <v>132</v>
@@ -3734,12 +3750,12 @@
     <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A50" s="19"/>
       <c r="B50" s="8"/>
-      <c r="C50" s="68"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="69"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="59"/>
+      <c r="H50" s="60"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8" t="s">
         <v>133</v>
@@ -3752,12 +3768,12 @@
     <row r="51" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="19"/>
       <c r="B51" s="8"/>
-      <c r="C51" s="68"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="51"/>
-      <c r="H51" s="69"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="59"/>
+      <c r="H51" s="60"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
       <c r="K51" s="21"/>
@@ -3768,12 +3784,12 @@
     <row r="52" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="19"/>
       <c r="B52" s="8"/>
-      <c r="C52" s="70"/>
-      <c r="D52" s="71"/>
-      <c r="E52" s="71"/>
-      <c r="F52" s="71"/>
-      <c r="G52" s="71"/>
-      <c r="H52" s="72"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="63"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
       <c r="K52" s="21"/>
@@ -3798,10 +3814,10 @@
     </row>
     <row r="56" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="57" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C57" s="56" t="s">
+      <c r="C57" s="46" t="s">
         <v>375</v>
       </c>
-      <c r="D57" s="57"/>
+      <c r="D57" s="47"/>
       <c r="F57" s="1" t="s">
         <v>376</v>
       </c>
@@ -3821,10 +3837,10 @@
       </c>
     </row>
     <row r="59" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C59" s="56" t="s">
+      <c r="C59" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="D59" s="57"/>
+      <c r="D59" s="47"/>
       <c r="F59" t="s">
         <v>44</v>
       </c>
@@ -3868,10 +3884,10 @@
       </c>
     </row>
     <row r="61" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C61" s="56" t="s">
+      <c r="C61" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="D61" s="57"/>
+      <c r="D61" s="47"/>
       <c r="O61" s="4" t="s">
         <v>74</v>
       </c>
@@ -3889,10 +3905,10 @@
       </c>
     </row>
     <row r="63" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C63" s="56" t="s">
+      <c r="C63" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="D63" s="57"/>
+      <c r="D63" s="47"/>
       <c r="O63" s="5" t="s">
         <v>75</v>
       </c>
@@ -3907,19 +3923,19 @@
       <c r="M64" t="s">
         <v>336</v>
       </c>
-      <c r="O64" s="56" t="s">
+      <c r="O64" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="P64" s="57"/>
+      <c r="P64" s="47"/>
       <c r="Q64" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="65" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C65" s="56" t="s">
+      <c r="C65" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="D65" s="57"/>
+      <c r="D65" s="47"/>
       <c r="Q65" t="s">
         <v>77</v>
       </c>
@@ -3930,10 +3946,10 @@
       </c>
     </row>
     <row r="67" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C67" s="56" t="s">
+      <c r="C67" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="D67" s="57"/>
+      <c r="D67" s="47"/>
       <c r="F67" s="15"/>
       <c r="G67" s="17"/>
       <c r="H67" s="17"/>
@@ -3964,10 +3980,10 @@
       </c>
     </row>
     <row r="69" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C69" s="56" t="s">
+      <c r="C69" s="46" t="s">
         <v>312</v>
       </c>
-      <c r="D69" s="57"/>
+      <c r="D69" s="47"/>
       <c r="F69" s="19"/>
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
@@ -4125,10 +4141,10 @@
       <c r="P75" t="s">
         <v>379</v>
       </c>
-      <c r="R75" s="56" t="s">
+      <c r="R75" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="S75" s="57"/>
+      <c r="S75" s="47"/>
       <c r="T75" t="s">
         <v>380</v>
       </c>
@@ -4149,10 +4165,10 @@
       <c r="P77" t="s">
         <v>336</v>
       </c>
-      <c r="R77" s="56" t="s">
+      <c r="R77" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="S77" s="57"/>
+      <c r="S77" s="47"/>
       <c r="T77" t="s">
         <v>381</v>
       </c>
@@ -4584,10 +4600,10 @@
     </row>
     <row r="125" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="126" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C126" s="56" t="s">
+      <c r="C126" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="D126" s="57"/>
+      <c r="D126" s="47"/>
       <c r="F126" t="s">
         <v>28</v>
       </c>
@@ -4618,10 +4634,10 @@
     </row>
     <row r="127" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="128" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C128" s="56" t="s">
+      <c r="C128" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="D128" s="57"/>
+      <c r="D128" s="47"/>
       <c r="N128" s="2" t="s">
         <v>108</v>
       </c>
@@ -4957,10 +4973,10 @@
       <c r="E160" s="19"/>
       <c r="F160" s="8"/>
       <c r="G160" s="8"/>
-      <c r="H160" s="59" t="s">
+      <c r="H160" s="48" t="s">
         <v>390</v>
       </c>
-      <c r="I160" s="60"/>
+      <c r="I160" s="49"/>
       <c r="J160" s="8"/>
       <c r="K160" s="21"/>
     </row>
@@ -4968,8 +4984,8 @@
       <c r="E161" s="19"/>
       <c r="F161" s="8"/>
       <c r="G161" s="8"/>
-      <c r="H161" s="61"/>
-      <c r="I161" s="62"/>
+      <c r="H161" s="50"/>
+      <c r="I161" s="51"/>
       <c r="J161" s="8"/>
       <c r="K161" s="21"/>
     </row>
@@ -4977,8 +4993,8 @@
       <c r="E162" s="19"/>
       <c r="F162" s="8"/>
       <c r="G162" s="8"/>
-      <c r="H162" s="61"/>
-      <c r="I162" s="62"/>
+      <c r="H162" s="50"/>
+      <c r="I162" s="51"/>
       <c r="J162" s="8"/>
       <c r="K162" s="21"/>
     </row>
@@ -4986,8 +5002,8 @@
       <c r="E163" s="19"/>
       <c r="F163" s="8"/>
       <c r="G163" s="8"/>
-      <c r="H163" s="61"/>
-      <c r="I163" s="62"/>
+      <c r="H163" s="50"/>
+      <c r="I163" s="51"/>
       <c r="J163" s="8"/>
       <c r="K163" s="21"/>
     </row>
@@ -4995,8 +5011,8 @@
       <c r="E164" s="19"/>
       <c r="F164" s="8"/>
       <c r="G164" s="8"/>
-      <c r="H164" s="63"/>
-      <c r="I164" s="64"/>
+      <c r="H164" s="52"/>
+      <c r="I164" s="53"/>
       <c r="J164" s="8"/>
       <c r="K164" s="21"/>
     </row>
@@ -5117,6 +5133,23 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="AL27:AN29"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="B5:C8"/>
+    <mergeCell ref="E5:F8"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C49:H52"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H29:J29"/>
     <mergeCell ref="R75:S75"/>
     <mergeCell ref="R77:S77"/>
     <mergeCell ref="H160:I164"/>
@@ -5128,23 +5161,6 @@
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="O64:P64"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B5:C8"/>
-    <mergeCell ref="E5:F8"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C49:H52"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="AL27:AN29"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="V32:W32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5432,16 +5448,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G14"/>
+  <dimension ref="A2:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
@@ -5704,6 +5720,29 @@
       </c>
       <c r="F14" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" t="s">
+        <v>416</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>417</v>
+      </c>
+      <c r="F15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -6235,7 +6274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>